<commit_message>
fixing the terminal output to be more useful
</commit_message>
<xml_diff>
--- a/Data/timings_Pd_2-4_treatments.xlsx
+++ b/Data/timings_Pd_2-4_treatments.xlsx
@@ -8,13 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Data Set 1 Timings" sheetId="1" r:id="rId1"/>
+    <sheet name="Data Set 2 Timings" sheetId="2" r:id="rId2"/>
+    <sheet name="Data Set 3 Timings" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="9">
   <si>
     <t>T_n</t>
   </si>
@@ -444,25 +446,25 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>0.23</v>
+        <v>0.17</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="F2">
-        <v>0.07000000000000001</v>
+        <v>0.052</v>
       </c>
       <c r="G2">
-        <v>0.06</v>
+        <v>0.043</v>
       </c>
       <c r="H2">
-        <v>0.05</v>
+        <v>0.041</v>
       </c>
       <c r="I2">
         <v>1000</v>
       </c>
       <c r="J2">
-        <v>3e-05</v>
+        <v>4e-05</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -476,25 +478,25 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>0.19</v>
+        <v>0.145</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="F3">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="G3">
-        <v>0.06</v>
+        <v>0.041</v>
       </c>
       <c r="H3">
-        <v>0.06</v>
+        <v>0.044</v>
       </c>
       <c r="I3">
         <v>1000</v>
       </c>
       <c r="J3">
-        <v>3e-05</v>
+        <v>2e-05</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -508,25 +510,25 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>0.19</v>
+        <v>0.145</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="F4">
-        <v>0.06</v>
+        <v>0.052</v>
       </c>
       <c r="G4">
-        <v>0.06</v>
+        <v>0.042</v>
       </c>
       <c r="H4">
-        <v>0.06</v>
+        <v>0.043</v>
       </c>
       <c r="I4">
         <v>1000</v>
       </c>
       <c r="J4">
-        <v>3e-05</v>
+        <v>2e-05</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -540,25 +542,25 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>0.19</v>
+        <v>0.145</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="F5">
-        <v>0.07000000000000001</v>
+        <v>0.052</v>
       </c>
       <c r="G5">
-        <v>0.06</v>
+        <v>0.042</v>
       </c>
       <c r="H5">
-        <v>0.05</v>
+        <v>0.042</v>
       </c>
       <c r="I5">
         <v>1000</v>
       </c>
       <c r="J5">
-        <v>3e-05</v>
+        <v>2e-05</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -572,25 +574,25 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>0.19</v>
+        <v>0.147</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="F6">
-        <v>0.06</v>
+        <v>0.054</v>
       </c>
       <c r="G6">
-        <v>0.06</v>
+        <v>0.043</v>
       </c>
       <c r="H6">
-        <v>0.06</v>
+        <v>0.041</v>
       </c>
       <c r="I6">
         <v>1000</v>
       </c>
       <c r="J6">
-        <v>3e-05</v>
+        <v>2e-05</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -604,25 +606,25 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>0.59</v>
+        <v>0.479</v>
       </c>
       <c r="E7">
-        <v>0.01</v>
+        <v>0.007</v>
       </c>
       <c r="F7">
-        <v>0.27</v>
+        <v>0.222</v>
       </c>
       <c r="G7">
-        <v>0.15</v>
+        <v>0.121</v>
       </c>
       <c r="H7">
-        <v>0.15</v>
+        <v>0.117</v>
       </c>
       <c r="I7">
         <v>1000</v>
       </c>
       <c r="J7">
-        <v>6.999999999999999e-05</v>
+        <v>2e-05</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -636,19 +638,19 @@
         <v>2</v>
       </c>
       <c r="D8">
-        <v>0.59</v>
+        <v>0.476</v>
       </c>
       <c r="E8">
-        <v>0.01</v>
+        <v>0.007</v>
       </c>
       <c r="F8">
-        <v>0.27</v>
+        <v>0.219</v>
       </c>
       <c r="G8">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="H8">
-        <v>0.15</v>
+        <v>0.118</v>
       </c>
       <c r="I8">
         <v>1000</v>
@@ -668,25 +670,25 @@
         <v>3</v>
       </c>
       <c r="D9">
-        <v>0.6</v>
+        <v>0.478</v>
       </c>
       <c r="E9">
-        <v>0.01</v>
+        <v>0.007</v>
       </c>
       <c r="F9">
-        <v>0.26</v>
+        <v>0.219</v>
       </c>
       <c r="G9">
-        <v>0.16</v>
+        <v>0.119</v>
       </c>
       <c r="H9">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="I9">
         <v>1000</v>
       </c>
       <c r="J9">
-        <v>6.999999999999999e-05</v>
+        <v>6e-05</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -700,25 +702,25 @@
         <v>4</v>
       </c>
       <c r="D10">
-        <v>0.6</v>
+        <v>0.487</v>
       </c>
       <c r="E10">
-        <v>0.01</v>
+        <v>0.007</v>
       </c>
       <c r="F10">
-        <v>0.27</v>
+        <v>0.232</v>
       </c>
       <c r="G10">
-        <v>0.15</v>
+        <v>0.119</v>
       </c>
       <c r="H10">
-        <v>0.16</v>
+        <v>0.117</v>
       </c>
       <c r="I10">
         <v>1000</v>
       </c>
       <c r="J10">
-        <v>6.999999999999999e-05</v>
+        <v>5e-05</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -732,25 +734,749 @@
         <v>5</v>
       </c>
       <c r="D11">
-        <v>0.59</v>
+        <v>0.478</v>
       </c>
       <c r="E11">
-        <v>0.01</v>
+        <v>0.007</v>
       </c>
       <c r="F11">
-        <v>0.26</v>
+        <v>0.223</v>
       </c>
       <c r="G11">
-        <v>0.16</v>
+        <v>0.118</v>
       </c>
       <c r="H11">
+        <v>0.118</v>
+      </c>
+      <c r="I11">
+        <v>1000</v>
+      </c>
+      <c r="J11">
+        <v>6e-05</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>0.15</v>
+      </c>
+      <c r="E2">
+        <v>0.002</v>
+      </c>
+      <c r="F2">
+        <v>0.056</v>
+      </c>
+      <c r="G2">
+        <v>0.043</v>
+      </c>
+      <c r="H2">
+        <v>0.042</v>
+      </c>
+      <c r="I2">
+        <v>1000</v>
+      </c>
+      <c r="J2">
+        <v>3e-05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>0.148</v>
+      </c>
+      <c r="E3">
+        <v>0.002</v>
+      </c>
+      <c r="F3">
+        <v>0.052</v>
+      </c>
+      <c r="G3">
+        <v>0.044</v>
+      </c>
+      <c r="H3">
+        <v>0.043</v>
+      </c>
+      <c r="I3">
+        <v>1000</v>
+      </c>
+      <c r="J3">
+        <v>1e-05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>0.147</v>
+      </c>
+      <c r="E4">
+        <v>0.002</v>
+      </c>
+      <c r="F4">
+        <v>0.052</v>
+      </c>
+      <c r="G4">
+        <v>0.043</v>
+      </c>
+      <c r="H4">
+        <v>0.043</v>
+      </c>
+      <c r="I4">
+        <v>1000</v>
+      </c>
+      <c r="J4">
+        <v>4e-05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>0.153</v>
+      </c>
+      <c r="E5">
+        <v>0.002</v>
+      </c>
+      <c r="F5">
+        <v>0.055</v>
+      </c>
+      <c r="G5">
+        <v>0.047</v>
+      </c>
+      <c r="H5">
+        <v>0.043</v>
+      </c>
+      <c r="I5">
+        <v>1000</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>0.147</v>
+      </c>
+      <c r="E6">
+        <v>0.001</v>
+      </c>
+      <c r="F6">
+        <v>0.055</v>
+      </c>
+      <c r="G6">
+        <v>0.043</v>
+      </c>
+      <c r="H6">
+        <v>0.042</v>
+      </c>
+      <c r="I6">
+        <v>1000</v>
+      </c>
+      <c r="J6">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0.479</v>
+      </c>
+      <c r="E7">
+        <v>0.007</v>
+      </c>
+      <c r="F7">
+        <v>0.222</v>
+      </c>
+      <c r="G7">
+        <v>0.121</v>
+      </c>
+      <c r="H7">
+        <v>0.116</v>
+      </c>
+      <c r="I7">
+        <v>1000</v>
+      </c>
+      <c r="J7">
+        <v>3e-05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>0.471</v>
+      </c>
+      <c r="E8">
+        <v>0.007</v>
+      </c>
+      <c r="F8">
+        <v>0.215</v>
+      </c>
+      <c r="G8">
+        <v>0.12</v>
+      </c>
+      <c r="H8">
+        <v>0.116</v>
+      </c>
+      <c r="I8">
+        <v>1000</v>
+      </c>
+      <c r="J8">
+        <v>6e-05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>0.475</v>
+      </c>
+      <c r="E9">
+        <v>0.007</v>
+      </c>
+      <c r="F9">
+        <v>0.22</v>
+      </c>
+      <c r="G9">
+        <v>0.117</v>
+      </c>
+      <c r="H9">
+        <v>0.118</v>
+      </c>
+      <c r="I9">
+        <v>1000</v>
+      </c>
+      <c r="J9">
+        <v>8.000000000000001e-05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>0.477</v>
+      </c>
+      <c r="E10">
+        <v>0.007</v>
+      </c>
+      <c r="F10">
+        <v>0.223</v>
+      </c>
+      <c r="G10">
+        <v>0.118</v>
+      </c>
+      <c r="H10">
+        <v>0.117</v>
+      </c>
+      <c r="I10">
+        <v>1000</v>
+      </c>
+      <c r="J10">
+        <v>8.000000000000001e-05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>0.478</v>
+      </c>
+      <c r="E11">
+        <v>0.007</v>
+      </c>
+      <c r="F11">
+        <v>0.223</v>
+      </c>
+      <c r="G11">
+        <v>0.118</v>
+      </c>
+      <c r="H11">
+        <v>0.118</v>
       </c>
       <c r="I11">
         <v>1000</v>
       </c>
       <c r="J11">
         <v>6.999999999999999e-05</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0.143</v>
+      </c>
+      <c r="E2">
+        <v>0.002</v>
+      </c>
+      <c r="F2">
+        <v>0.051</v>
+      </c>
+      <c r="G2">
+        <v>0.043</v>
+      </c>
+      <c r="H2">
+        <v>0.042</v>
+      </c>
+      <c r="I2">
+        <v>1000</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>0.147</v>
+      </c>
+      <c r="E3">
+        <v>0.002</v>
+      </c>
+      <c r="F3">
+        <v>0.052</v>
+      </c>
+      <c r="G3">
+        <v>0.044</v>
+      </c>
+      <c r="H3">
+        <v>0.043</v>
+      </c>
+      <c r="I3">
+        <v>1000</v>
+      </c>
+      <c r="J3">
+        <v>5e-05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>0.145</v>
+      </c>
+      <c r="E4">
+        <v>0.001</v>
+      </c>
+      <c r="F4">
+        <v>0.052</v>
+      </c>
+      <c r="G4">
+        <v>0.043</v>
+      </c>
+      <c r="H4">
+        <v>0.042</v>
+      </c>
+      <c r="I4">
+        <v>1000</v>
+      </c>
+      <c r="J4">
+        <v>3e-05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>0.145</v>
+      </c>
+      <c r="E5">
+        <v>0.002</v>
+      </c>
+      <c r="F5">
+        <v>0.052</v>
+      </c>
+      <c r="G5">
+        <v>0.043</v>
+      </c>
+      <c r="H5">
+        <v>0.043</v>
+      </c>
+      <c r="I5">
+        <v>1000</v>
+      </c>
+      <c r="J5">
+        <v>5e-05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>0.148</v>
+      </c>
+      <c r="E6">
+        <v>0.002</v>
+      </c>
+      <c r="F6">
+        <v>0.056</v>
+      </c>
+      <c r="G6">
+        <v>0.043</v>
+      </c>
+      <c r="H6">
+        <v>0.041</v>
+      </c>
+      <c r="I6">
+        <v>1000</v>
+      </c>
+      <c r="J6">
+        <v>4e-05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0.477</v>
+      </c>
+      <c r="E7">
+        <v>0.007</v>
+      </c>
+      <c r="F7">
+        <v>0.221</v>
+      </c>
+      <c r="G7">
+        <v>0.121</v>
+      </c>
+      <c r="H7">
+        <v>0.116</v>
+      </c>
+      <c r="I7">
+        <v>1000</v>
+      </c>
+      <c r="J7">
+        <v>5e-05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>0.512</v>
+      </c>
+      <c r="E8">
+        <v>0.007</v>
+      </c>
+      <c r="F8">
+        <v>0.217</v>
+      </c>
+      <c r="G8">
+        <v>0.16</v>
+      </c>
+      <c r="H8">
+        <v>0.117</v>
+      </c>
+      <c r="I8">
+        <v>1000</v>
+      </c>
+      <c r="J8">
+        <v>6.999999999999999e-05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>0.478</v>
+      </c>
+      <c r="E9">
+        <v>0.007</v>
+      </c>
+      <c r="F9">
+        <v>0.222</v>
+      </c>
+      <c r="G9">
+        <v>0.118</v>
+      </c>
+      <c r="H9">
+        <v>0.119</v>
+      </c>
+      <c r="I9">
+        <v>1000</v>
+      </c>
+      <c r="J9">
+        <v>5e-05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>0.477</v>
+      </c>
+      <c r="E10">
+        <v>0.007</v>
+      </c>
+      <c r="F10">
+        <v>0.22</v>
+      </c>
+      <c r="G10">
+        <v>0.12</v>
+      </c>
+      <c r="H10">
+        <v>0.117</v>
+      </c>
+      <c r="I10">
+        <v>1000</v>
+      </c>
+      <c r="J10">
+        <v>8.000000000000001e-05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>0.483</v>
+      </c>
+      <c r="E11">
+        <v>0.008</v>
+      </c>
+      <c r="F11">
+        <v>0.227</v>
+      </c>
+      <c r="G11">
+        <v>0.118</v>
+      </c>
+      <c r="H11">
+        <v>0.118</v>
+      </c>
+      <c r="I11">
+        <v>1000</v>
+      </c>
+      <c r="J11">
+        <v>5e-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>